<commit_message>
supported LINKTEXT, CSS, and PARTIALLINKTEXT locators
</commit_message>
<xml_diff>
--- a/src/testdata/SampleTestData.xlsx
+++ b/src/testdata/SampleTestData.xlsx
@@ -2,17 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SeleniumProject\src\acn\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jed.v.colina\workspace\seleniumframework\src\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Sheet" sheetId="7" r:id="rId1"/>
+    <sheet name="DemoTours" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -45,12 +46,57 @@
   </si>
   <si>
     <t>http://google.com</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State/Province</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>DemoAutTest</t>
+  </si>
+  <si>
+    <t>Jed</t>
+  </si>
+  <si>
+    <t>http://www.newtours.demoaut.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -160,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -198,6 +244,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,9 +528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FR3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,4 +1359,688 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:FR3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.5703125" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" customWidth="1"/>
+    <col min="25" max="25" width="11.5703125" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" customWidth="1"/>
+    <col min="27" max="27" width="8.7109375" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" customWidth="1"/>
+    <col min="30" max="30" width="19.42578125" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" customWidth="1"/>
+    <col min="32" max="32" width="19.85546875" customWidth="1"/>
+    <col min="33" max="33" width="8.7109375" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" customWidth="1"/>
+    <col min="36" max="36" width="18.85546875" customWidth="1"/>
+    <col min="37" max="37" width="11.5703125" customWidth="1"/>
+    <col min="38" max="38" width="17.42578125" customWidth="1"/>
+    <col min="39" max="39" width="8.7109375" customWidth="1"/>
+    <col min="40" max="40" width="12.28515625" customWidth="1"/>
+    <col min="41" max="41" width="16.85546875" customWidth="1"/>
+    <col min="42" max="42" width="19.140625" customWidth="1"/>
+    <col min="43" max="43" width="11.5703125" customWidth="1"/>
+    <col min="44" max="44" width="19.140625" customWidth="1"/>
+    <col min="45" max="45" width="8.7109375" customWidth="1"/>
+    <col min="46" max="46" width="12.28515625" customWidth="1"/>
+    <col min="47" max="47" width="14.28515625" customWidth="1"/>
+    <col min="48" max="48" width="16.85546875" customWidth="1"/>
+    <col min="49" max="49" width="18.85546875" customWidth="1"/>
+    <col min="50" max="50" width="11.5703125" customWidth="1"/>
+    <col min="51" max="51" width="18.85546875" customWidth="1"/>
+    <col min="52" max="52" width="8.7109375" customWidth="1"/>
+    <col min="53" max="53" width="12.28515625" customWidth="1"/>
+    <col min="54" max="54" width="14.28515625" customWidth="1"/>
+    <col min="55" max="55" width="16.85546875" customWidth="1"/>
+    <col min="56" max="56" width="18.85546875" customWidth="1"/>
+    <col min="57" max="57" width="11.5703125" customWidth="1"/>
+    <col min="58" max="58" width="18.85546875" customWidth="1"/>
+    <col min="59" max="59" width="8.7109375" customWidth="1"/>
+    <col min="60" max="60" width="12.28515625" customWidth="1"/>
+    <col min="61" max="61" width="14.28515625" customWidth="1"/>
+    <col min="62" max="62" width="16.85546875" customWidth="1"/>
+    <col min="63" max="63" width="18.85546875" customWidth="1"/>
+    <col min="64" max="64" width="11.5703125" customWidth="1"/>
+    <col min="65" max="66" width="18.85546875" customWidth="1"/>
+    <col min="67" max="67" width="8.7109375" customWidth="1"/>
+    <col min="68" max="68" width="12.28515625" customWidth="1"/>
+    <col min="69" max="76" width="20.7109375" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" customWidth="1"/>
+    <col min="78" max="92" width="3" customWidth="1"/>
+    <col min="93" max="99" width="16.42578125" customWidth="1"/>
+    <col min="100" max="100" width="12.42578125" customWidth="1"/>
+    <col min="101" max="101" width="18.42578125" customWidth="1"/>
+    <col min="102" max="102" width="16.140625" customWidth="1"/>
+    <col min="103" max="103" width="15.5703125" customWidth="1"/>
+    <col min="104" max="105" width="14.28515625" customWidth="1"/>
+    <col min="110" max="110" width="18.42578125" customWidth="1"/>
+    <col min="111" max="111" width="14.85546875" customWidth="1"/>
+    <col min="113" max="113" width="11.42578125" customWidth="1"/>
+    <col min="114" max="114" width="12.5703125" customWidth="1"/>
+    <col min="117" max="117" width="11" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="12.7109375" customWidth="1"/>
+    <col min="121" max="121" width="16.85546875" customWidth="1"/>
+    <col min="126" max="126" width="11.42578125" customWidth="1"/>
+    <col min="128" max="128" width="13.42578125" customWidth="1"/>
+    <col min="129" max="129" width="12.5703125" customWidth="1"/>
+    <col min="130" max="130" width="12" customWidth="1"/>
+    <col min="131" max="131" width="10" customWidth="1"/>
+    <col min="137" max="137" width="10.85546875" customWidth="1"/>
+    <col min="138" max="138" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:174" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>45</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="1">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="1">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="1">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="1">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="1">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="1">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="1">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="1">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="1">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="1">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="1">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="1">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="1">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="1">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="1">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="1">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="1">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="1">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="1">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="1">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="1">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="1">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="1">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="1">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="1"/>
+      <c r="CP1" s="1"/>
+      <c r="CQ1" s="1"/>
+      <c r="CR1" s="1"/>
+      <c r="CS1" s="1"/>
+      <c r="CT1" s="1"/>
+      <c r="CU1" s="1"/>
+      <c r="CV1" s="1"/>
+      <c r="CW1" s="1"/>
+      <c r="CX1" s="1"/>
+      <c r="CY1" s="1"/>
+      <c r="CZ1" s="1"/>
+      <c r="DA1" s="1"/>
+      <c r="DB1" s="1"/>
+      <c r="DC1" s="1"/>
+      <c r="DD1" s="1"/>
+      <c r="DE1" s="1"/>
+      <c r="DF1" s="1"/>
+      <c r="DG1" s="1"/>
+      <c r="DH1" s="1"/>
+      <c r="DI1" s="1"/>
+      <c r="DJ1" s="1"/>
+      <c r="DK1" s="1"/>
+      <c r="DL1" s="1"/>
+      <c r="DM1" s="1"/>
+      <c r="DN1" s="1"/>
+      <c r="DO1" s="1"/>
+      <c r="DP1" s="1"/>
+      <c r="DQ1" s="1"/>
+      <c r="DR1" s="1"/>
+      <c r="DS1" s="1"/>
+      <c r="DT1" s="1"/>
+      <c r="DU1" s="1"/>
+      <c r="DV1" s="1"/>
+      <c r="DW1" s="1"/>
+      <c r="DX1" s="1"/>
+      <c r="DY1" s="1"/>
+      <c r="DZ1" s="1"/>
+      <c r="EA1" s="1"/>
+      <c r="EB1" s="1"/>
+      <c r="EC1" s="1"/>
+      <c r="ED1" s="1"/>
+      <c r="EE1" s="1"/>
+      <c r="EF1" s="1"/>
+      <c r="EG1" s="1"/>
+      <c r="EH1" s="1"/>
+      <c r="EI1" s="1"/>
+      <c r="EJ1" s="1"/>
+      <c r="EK1" s="1"/>
+      <c r="EL1" s="1"/>
+      <c r="EM1" s="1"/>
+      <c r="EN1" s="1"/>
+      <c r="EO1" s="1"/>
+      <c r="EP1" s="1"/>
+      <c r="EQ1" s="1"/>
+      <c r="ER1" s="1"/>
+      <c r="ES1" s="1"/>
+      <c r="ET1" s="1"/>
+      <c r="EU1" s="1"/>
+      <c r="EV1" s="1"/>
+      <c r="EW1" s="1"/>
+      <c r="EX1" s="1"/>
+      <c r="EY1" s="1"/>
+      <c r="EZ1" s="1"/>
+      <c r="FA1" s="1"/>
+      <c r="FB1" s="1"/>
+      <c r="FC1" s="1"/>
+      <c r="FD1" s="1"/>
+      <c r="FE1" s="1"/>
+      <c r="FF1" s="1"/>
+      <c r="FG1" s="1"/>
+      <c r="FH1" s="1"/>
+      <c r="FI1" s="1"/>
+      <c r="FJ1" s="1"/>
+      <c r="FK1" s="1"/>
+      <c r="FL1" s="1"/>
+      <c r="FM1" s="1"/>
+      <c r="FN1" s="1"/>
+      <c r="FO1" s="1"/>
+      <c r="FP1" s="1"/>
+    </row>
+    <row r="2" spans="1:174" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9"/>
+      <c r="BK2" s="9"/>
+      <c r="BL2" s="9"/>
+      <c r="BM2" s="9"/>
+      <c r="BN2" s="9"/>
+      <c r="BO2" s="9"/>
+      <c r="BP2" s="9"/>
+      <c r="BQ2" s="9"/>
+      <c r="BR2" s="9"/>
+      <c r="BS2" s="9"/>
+      <c r="BT2" s="9"/>
+      <c r="BU2" s="9"/>
+      <c r="BV2" s="9"/>
+      <c r="BW2" s="9"/>
+      <c r="BX2" s="9"/>
+      <c r="BY2" s="9"/>
+      <c r="BZ2" s="9"/>
+      <c r="CA2" s="9"/>
+      <c r="CB2" s="9"/>
+      <c r="CC2" s="9"/>
+      <c r="CD2" s="9"/>
+      <c r="CE2" s="9"/>
+      <c r="CF2" s="9"/>
+      <c r="CG2" s="9"/>
+      <c r="CH2" s="9"/>
+      <c r="CI2" s="9"/>
+      <c r="CJ2" s="9"/>
+      <c r="CK2" s="9"/>
+      <c r="CL2" s="9"/>
+      <c r="CM2" s="9"/>
+      <c r="CN2" s="9"/>
+      <c r="CO2" s="9"/>
+      <c r="CP2" s="9"/>
+      <c r="CQ2" s="9"/>
+      <c r="CR2" s="9"/>
+      <c r="CS2" s="9"/>
+      <c r="CT2" s="9"/>
+      <c r="CU2" s="9"/>
+      <c r="CV2" s="9"/>
+      <c r="CW2" s="9"/>
+      <c r="CX2" s="9"/>
+      <c r="CY2" s="9"/>
+      <c r="CZ2" s="9"/>
+      <c r="DA2" s="9"/>
+      <c r="DB2" s="9"/>
+      <c r="DC2" s="9"/>
+      <c r="DD2" s="9"/>
+      <c r="DE2" s="9"/>
+      <c r="DF2" s="9"/>
+      <c r="DG2" s="9"/>
+      <c r="DH2" s="9"/>
+      <c r="DI2" s="9"/>
+      <c r="DJ2" s="9"/>
+      <c r="DK2" s="9"/>
+      <c r="DL2" s="9"/>
+      <c r="DM2" s="9"/>
+      <c r="DN2" s="9"/>
+      <c r="DO2" s="9"/>
+      <c r="DP2" s="9"/>
+      <c r="DQ2" s="9"/>
+      <c r="DR2" s="9"/>
+      <c r="DS2" s="9"/>
+      <c r="DT2" s="9"/>
+      <c r="DU2" s="9"/>
+      <c r="DV2" s="9"/>
+      <c r="DW2" s="9"/>
+      <c r="DX2" s="9"/>
+      <c r="DY2" s="9"/>
+      <c r="DZ2" s="9"/>
+      <c r="EA2" s="9"/>
+      <c r="EB2" s="9"/>
+      <c r="EC2" s="9"/>
+      <c r="ED2" s="9"/>
+      <c r="EE2" s="9"/>
+      <c r="EF2" s="9"/>
+      <c r="EG2" s="9"/>
+      <c r="EH2" s="9"/>
+      <c r="EI2" s="9"/>
+      <c r="EJ2" s="9"/>
+      <c r="EK2" s="9"/>
+      <c r="EL2" s="9"/>
+      <c r="EM2" s="9"/>
+      <c r="EN2" s="9"/>
+      <c r="EO2" s="9"/>
+      <c r="EP2" s="9"/>
+      <c r="EQ2" s="9"/>
+      <c r="ER2" s="9"/>
+      <c r="ES2" s="9"/>
+      <c r="ET2" s="9"/>
+      <c r="EU2" s="9"/>
+      <c r="EV2" s="9"/>
+      <c r="EW2" s="9"/>
+      <c r="EX2" s="9"/>
+      <c r="EY2" s="9"/>
+      <c r="EZ2" s="9"/>
+      <c r="FA2" s="9"/>
+      <c r="FB2" s="9"/>
+      <c r="FC2" s="9"/>
+      <c r="FD2" s="9"/>
+      <c r="FE2" s="9"/>
+      <c r="FF2" s="9"/>
+      <c r="FG2" s="9"/>
+      <c r="FH2" s="9"/>
+      <c r="FI2" s="9"/>
+      <c r="FJ2" s="9"/>
+      <c r="FK2" s="9"/>
+      <c r="FL2" s="9"/>
+      <c r="FM2" s="9"/>
+      <c r="FN2" s="9"/>
+      <c r="FO2" s="9"/>
+      <c r="FP2" s="9"/>
+      <c r="FQ2" s="9"/>
+      <c r="FR2" s="9"/>
+    </row>
+    <row r="3" spans="1:174" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
started fixing design issues with the framework
</commit_message>
<xml_diff>
--- a/src/testdata/SampleTestData.xlsx
+++ b/src/testdata/SampleTestData.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Sheet" sheetId="7" r:id="rId1"/>
-    <sheet name="DemoTours" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -48,49 +47,7 @@
     <t>http://google.com</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State/Province</t>
-  </si>
-  <si>
-    <t>Postal Code</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>User Name</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Confirm Password</t>
-  </si>
-  <si>
-    <t>DemoAutTest</t>
-  </si>
-  <si>
-    <t>Jed</t>
-  </si>
-  <si>
-    <t>http://www.newtours.demoaut.com/</t>
+    <t>Banana</t>
   </si>
 </sst>
 </file>
@@ -206,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -244,7 +201,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -528,9 +484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FR3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +940,7 @@
       <c r="FO1" s="1"/>
       <c r="FP1" s="1"/>
     </row>
-    <row r="2" spans="1:174" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:174" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -997,8 +953,12 @@
       <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -1181,8 +1141,12 @@
       <c r="D3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1359,688 +1323,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FR3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" customWidth="1"/>
-    <col min="24" max="24" width="18.85546875" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" customWidth="1"/>
-    <col min="26" max="26" width="20.42578125" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" customWidth="1"/>
-    <col min="28" max="28" width="12.28515625" customWidth="1"/>
-    <col min="29" max="29" width="16.85546875" customWidth="1"/>
-    <col min="30" max="30" width="19.42578125" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" customWidth="1"/>
-    <col min="32" max="32" width="19.85546875" customWidth="1"/>
-    <col min="33" max="33" width="8.7109375" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" customWidth="1"/>
-    <col min="35" max="35" width="16.85546875" customWidth="1"/>
-    <col min="36" max="36" width="18.85546875" customWidth="1"/>
-    <col min="37" max="37" width="11.5703125" customWidth="1"/>
-    <col min="38" max="38" width="17.42578125" customWidth="1"/>
-    <col min="39" max="39" width="8.7109375" customWidth="1"/>
-    <col min="40" max="40" width="12.28515625" customWidth="1"/>
-    <col min="41" max="41" width="16.85546875" customWidth="1"/>
-    <col min="42" max="42" width="19.140625" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" customWidth="1"/>
-    <col min="44" max="44" width="19.140625" customWidth="1"/>
-    <col min="45" max="45" width="8.7109375" customWidth="1"/>
-    <col min="46" max="46" width="12.28515625" customWidth="1"/>
-    <col min="47" max="47" width="14.28515625" customWidth="1"/>
-    <col min="48" max="48" width="16.85546875" customWidth="1"/>
-    <col min="49" max="49" width="18.85546875" customWidth="1"/>
-    <col min="50" max="50" width="11.5703125" customWidth="1"/>
-    <col min="51" max="51" width="18.85546875" customWidth="1"/>
-    <col min="52" max="52" width="8.7109375" customWidth="1"/>
-    <col min="53" max="53" width="12.28515625" customWidth="1"/>
-    <col min="54" max="54" width="14.28515625" customWidth="1"/>
-    <col min="55" max="55" width="16.85546875" customWidth="1"/>
-    <col min="56" max="56" width="18.85546875" customWidth="1"/>
-    <col min="57" max="57" width="11.5703125" customWidth="1"/>
-    <col min="58" max="58" width="18.85546875" customWidth="1"/>
-    <col min="59" max="59" width="8.7109375" customWidth="1"/>
-    <col min="60" max="60" width="12.28515625" customWidth="1"/>
-    <col min="61" max="61" width="14.28515625" customWidth="1"/>
-    <col min="62" max="62" width="16.85546875" customWidth="1"/>
-    <col min="63" max="63" width="18.85546875" customWidth="1"/>
-    <col min="64" max="64" width="11.5703125" customWidth="1"/>
-    <col min="65" max="66" width="18.85546875" customWidth="1"/>
-    <col min="67" max="67" width="8.7109375" customWidth="1"/>
-    <col min="68" max="68" width="12.28515625" customWidth="1"/>
-    <col min="69" max="76" width="20.7109375" customWidth="1"/>
-    <col min="77" max="77" width="19.28515625" customWidth="1"/>
-    <col min="78" max="92" width="3" customWidth="1"/>
-    <col min="93" max="99" width="16.42578125" customWidth="1"/>
-    <col min="100" max="100" width="12.42578125" customWidth="1"/>
-    <col min="101" max="101" width="18.42578125" customWidth="1"/>
-    <col min="102" max="102" width="16.140625" customWidth="1"/>
-    <col min="103" max="103" width="15.5703125" customWidth="1"/>
-    <col min="104" max="105" width="14.28515625" customWidth="1"/>
-    <col min="110" max="110" width="18.42578125" customWidth="1"/>
-    <col min="111" max="111" width="14.85546875" customWidth="1"/>
-    <col min="113" max="113" width="11.42578125" customWidth="1"/>
-    <col min="114" max="114" width="12.5703125" customWidth="1"/>
-    <col min="117" max="117" width="11" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="12.7109375" customWidth="1"/>
-    <col min="121" max="121" width="16.85546875" customWidth="1"/>
-    <col min="126" max="126" width="11.42578125" customWidth="1"/>
-    <col min="128" max="128" width="13.42578125" customWidth="1"/>
-    <col min="129" max="129" width="12.5703125" customWidth="1"/>
-    <col min="130" max="130" width="12" customWidth="1"/>
-    <col min="131" max="131" width="10" customWidth="1"/>
-    <col min="137" max="137" width="10.85546875" customWidth="1"/>
-    <col min="138" max="138" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:174" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>38</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>39</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="1">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="1">
-        <v>42</v>
-      </c>
-      <c r="AR1" s="1">
-        <v>43</v>
-      </c>
-      <c r="AS1" s="1">
-        <v>44</v>
-      </c>
-      <c r="AT1" s="1">
-        <v>45</v>
-      </c>
-      <c r="AU1" s="1">
-        <v>46</v>
-      </c>
-      <c r="AV1" s="1">
-        <v>47</v>
-      </c>
-      <c r="AW1" s="1">
-        <v>48</v>
-      </c>
-      <c r="AX1" s="1">
-        <v>49</v>
-      </c>
-      <c r="AY1" s="1">
-        <v>50</v>
-      </c>
-      <c r="AZ1" s="1">
-        <v>51</v>
-      </c>
-      <c r="BA1" s="1">
-        <v>52</v>
-      </c>
-      <c r="BB1" s="1">
-        <v>53</v>
-      </c>
-      <c r="BC1" s="1">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="1">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="1">
-        <v>56</v>
-      </c>
-      <c r="BF1" s="1">
-        <v>57</v>
-      </c>
-      <c r="BG1" s="1">
-        <v>58</v>
-      </c>
-      <c r="BH1" s="1">
-        <v>59</v>
-      </c>
-      <c r="BI1" s="1">
-        <v>60</v>
-      </c>
-      <c r="BJ1" s="1">
-        <v>61</v>
-      </c>
-      <c r="BK1" s="1">
-        <v>62</v>
-      </c>
-      <c r="BL1" s="1">
-        <v>63</v>
-      </c>
-      <c r="BM1" s="1">
-        <v>64</v>
-      </c>
-      <c r="BN1" s="1">
-        <v>65</v>
-      </c>
-      <c r="BO1" s="1">
-        <v>66</v>
-      </c>
-      <c r="BP1" s="1">
-        <v>67</v>
-      </c>
-      <c r="BQ1" s="1">
-        <v>68</v>
-      </c>
-      <c r="BR1" s="1">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="1">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="1">
-        <v>71</v>
-      </c>
-      <c r="BU1" s="1">
-        <v>72</v>
-      </c>
-      <c r="BV1" s="1">
-        <v>73</v>
-      </c>
-      <c r="BW1" s="1">
-        <v>74</v>
-      </c>
-      <c r="BX1" s="1">
-        <v>75</v>
-      </c>
-      <c r="BY1" s="1">
-        <v>76</v>
-      </c>
-      <c r="BZ1" s="1">
-        <v>77</v>
-      </c>
-      <c r="CA1" s="1">
-        <v>78</v>
-      </c>
-      <c r="CB1" s="1">
-        <v>79</v>
-      </c>
-      <c r="CC1" s="1">
-        <v>80</v>
-      </c>
-      <c r="CD1" s="1">
-        <v>81</v>
-      </c>
-      <c r="CE1" s="1">
-        <v>82</v>
-      </c>
-      <c r="CF1" s="1">
-        <v>83</v>
-      </c>
-      <c r="CG1" s="1">
-        <v>84</v>
-      </c>
-      <c r="CH1" s="1">
-        <v>85</v>
-      </c>
-      <c r="CI1" s="1">
-        <v>86</v>
-      </c>
-      <c r="CJ1" s="1">
-        <v>87</v>
-      </c>
-      <c r="CK1" s="1">
-        <v>88</v>
-      </c>
-      <c r="CL1" s="1">
-        <v>89</v>
-      </c>
-      <c r="CM1" s="1">
-        <v>90</v>
-      </c>
-      <c r="CN1" s="1">
-        <v>91</v>
-      </c>
-      <c r="CO1" s="1"/>
-      <c r="CP1" s="1"/>
-      <c r="CQ1" s="1"/>
-      <c r="CR1" s="1"/>
-      <c r="CS1" s="1"/>
-      <c r="CT1" s="1"/>
-      <c r="CU1" s="1"/>
-      <c r="CV1" s="1"/>
-      <c r="CW1" s="1"/>
-      <c r="CX1" s="1"/>
-      <c r="CY1" s="1"/>
-      <c r="CZ1" s="1"/>
-      <c r="DA1" s="1"/>
-      <c r="DB1" s="1"/>
-      <c r="DC1" s="1"/>
-      <c r="DD1" s="1"/>
-      <c r="DE1" s="1"/>
-      <c r="DF1" s="1"/>
-      <c r="DG1" s="1"/>
-      <c r="DH1" s="1"/>
-      <c r="DI1" s="1"/>
-      <c r="DJ1" s="1"/>
-      <c r="DK1" s="1"/>
-      <c r="DL1" s="1"/>
-      <c r="DM1" s="1"/>
-      <c r="DN1" s="1"/>
-      <c r="DO1" s="1"/>
-      <c r="DP1" s="1"/>
-      <c r="DQ1" s="1"/>
-      <c r="DR1" s="1"/>
-      <c r="DS1" s="1"/>
-      <c r="DT1" s="1"/>
-      <c r="DU1" s="1"/>
-      <c r="DV1" s="1"/>
-      <c r="DW1" s="1"/>
-      <c r="DX1" s="1"/>
-      <c r="DY1" s="1"/>
-      <c r="DZ1" s="1"/>
-      <c r="EA1" s="1"/>
-      <c r="EB1" s="1"/>
-      <c r="EC1" s="1"/>
-      <c r="ED1" s="1"/>
-      <c r="EE1" s="1"/>
-      <c r="EF1" s="1"/>
-      <c r="EG1" s="1"/>
-      <c r="EH1" s="1"/>
-      <c r="EI1" s="1"/>
-      <c r="EJ1" s="1"/>
-      <c r="EK1" s="1"/>
-      <c r="EL1" s="1"/>
-      <c r="EM1" s="1"/>
-      <c r="EN1" s="1"/>
-      <c r="EO1" s="1"/>
-      <c r="EP1" s="1"/>
-      <c r="EQ1" s="1"/>
-      <c r="ER1" s="1"/>
-      <c r="ES1" s="1"/>
-      <c r="ET1" s="1"/>
-      <c r="EU1" s="1"/>
-      <c r="EV1" s="1"/>
-      <c r="EW1" s="1"/>
-      <c r="EX1" s="1"/>
-      <c r="EY1" s="1"/>
-      <c r="EZ1" s="1"/>
-      <c r="FA1" s="1"/>
-      <c r="FB1" s="1"/>
-      <c r="FC1" s="1"/>
-      <c r="FD1" s="1"/>
-      <c r="FE1" s="1"/>
-      <c r="FF1" s="1"/>
-      <c r="FG1" s="1"/>
-      <c r="FH1" s="1"/>
-      <c r="FI1" s="1"/>
-      <c r="FJ1" s="1"/>
-      <c r="FK1" s="1"/>
-      <c r="FL1" s="1"/>
-      <c r="FM1" s="1"/>
-      <c r="FN1" s="1"/>
-      <c r="FO1" s="1"/>
-      <c r="FP1" s="1"/>
-    </row>
-    <row r="2" spans="1:174" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9"/>
-      <c r="AP2" s="9"/>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="9"/>
-      <c r="BL2" s="9"/>
-      <c r="BM2" s="9"/>
-      <c r="BN2" s="9"/>
-      <c r="BO2" s="9"/>
-      <c r="BP2" s="9"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="9"/>
-      <c r="BS2" s="9"/>
-      <c r="BT2" s="9"/>
-      <c r="BU2" s="9"/>
-      <c r="BV2" s="9"/>
-      <c r="BW2" s="9"/>
-      <c r="BX2" s="9"/>
-      <c r="BY2" s="9"/>
-      <c r="BZ2" s="9"/>
-      <c r="CA2" s="9"/>
-      <c r="CB2" s="9"/>
-      <c r="CC2" s="9"/>
-      <c r="CD2" s="9"/>
-      <c r="CE2" s="9"/>
-      <c r="CF2" s="9"/>
-      <c r="CG2" s="9"/>
-      <c r="CH2" s="9"/>
-      <c r="CI2" s="9"/>
-      <c r="CJ2" s="9"/>
-      <c r="CK2" s="9"/>
-      <c r="CL2" s="9"/>
-      <c r="CM2" s="9"/>
-      <c r="CN2" s="9"/>
-      <c r="CO2" s="9"/>
-      <c r="CP2" s="9"/>
-      <c r="CQ2" s="9"/>
-      <c r="CR2" s="9"/>
-      <c r="CS2" s="9"/>
-      <c r="CT2" s="9"/>
-      <c r="CU2" s="9"/>
-      <c r="CV2" s="9"/>
-      <c r="CW2" s="9"/>
-      <c r="CX2" s="9"/>
-      <c r="CY2" s="9"/>
-      <c r="CZ2" s="9"/>
-      <c r="DA2" s="9"/>
-      <c r="DB2" s="9"/>
-      <c r="DC2" s="9"/>
-      <c r="DD2" s="9"/>
-      <c r="DE2" s="9"/>
-      <c r="DF2" s="9"/>
-      <c r="DG2" s="9"/>
-      <c r="DH2" s="9"/>
-      <c r="DI2" s="9"/>
-      <c r="DJ2" s="9"/>
-      <c r="DK2" s="9"/>
-      <c r="DL2" s="9"/>
-      <c r="DM2" s="9"/>
-      <c r="DN2" s="9"/>
-      <c r="DO2" s="9"/>
-      <c r="DP2" s="9"/>
-      <c r="DQ2" s="9"/>
-      <c r="DR2" s="9"/>
-      <c r="DS2" s="9"/>
-      <c r="DT2" s="9"/>
-      <c r="DU2" s="9"/>
-      <c r="DV2" s="9"/>
-      <c r="DW2" s="9"/>
-      <c r="DX2" s="9"/>
-      <c r="DY2" s="9"/>
-      <c r="DZ2" s="9"/>
-      <c r="EA2" s="9"/>
-      <c r="EB2" s="9"/>
-      <c r="EC2" s="9"/>
-      <c r="ED2" s="9"/>
-      <c r="EE2" s="9"/>
-      <c r="EF2" s="9"/>
-      <c r="EG2" s="9"/>
-      <c r="EH2" s="9"/>
-      <c r="EI2" s="9"/>
-      <c r="EJ2" s="9"/>
-      <c r="EK2" s="9"/>
-      <c r="EL2" s="9"/>
-      <c r="EM2" s="9"/>
-      <c r="EN2" s="9"/>
-      <c r="EO2" s="9"/>
-      <c r="EP2" s="9"/>
-      <c r="EQ2" s="9"/>
-      <c r="ER2" s="9"/>
-      <c r="ES2" s="9"/>
-      <c r="ET2" s="9"/>
-      <c r="EU2" s="9"/>
-      <c r="EV2" s="9"/>
-      <c r="EW2" s="9"/>
-      <c r="EX2" s="9"/>
-      <c r="EY2" s="9"/>
-      <c r="EZ2" s="9"/>
-      <c r="FA2" s="9"/>
-      <c r="FB2" s="9"/>
-      <c r="FC2" s="9"/>
-      <c r="FD2" s="9"/>
-      <c r="FE2" s="9"/>
-      <c r="FF2" s="9"/>
-      <c r="FG2" s="9"/>
-      <c r="FH2" s="9"/>
-      <c r="FI2" s="9"/>
-      <c r="FJ2" s="9"/>
-      <c r="FK2" s="9"/>
-      <c r="FL2" s="9"/>
-      <c r="FM2" s="9"/>
-      <c r="FN2" s="9"/>
-      <c r="FO2" s="9"/>
-      <c r="FP2" s="9"/>
-      <c r="FQ2" s="9"/>
-      <c r="FR2" s="9"/>
-    </row>
-    <row r="3" spans="1:174" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>